<commit_message>
Added salt to the master password. Implemented encryption for login entries derived from the master password including padding and salt. The algorithm used is AES - CBC mode. Implemented UI for the main form showing user's login pairs. and some other shite
</commit_message>
<xml_diff>
--- a/PassManager - Functionality.xlsx
+++ b/PassManager - Functionality.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JStol\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JStol\Desktop\PassManager_GitClone\PassManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDAAD7E-695A-41E3-95E4-98F7A12BF768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FFA341-7393-43E5-A725-FA65CF5A6BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{930275F6-655A-4A0B-862D-4D7EDAD07EBB}"/>
+    <workbookView xWindow="22932" yWindow="-8820" windowWidth="14616" windowHeight="22536" xr2:uid="{930275F6-655A-4A0B-862D-4D7EDAD07EBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Functionality Details" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t>Functionality</t>
   </si>
@@ -56,18 +56,12 @@
     <t>Form</t>
   </si>
   <si>
-    <t>Form1 (login)</t>
-  </si>
-  <si>
     <t>Form2 (main)</t>
   </si>
   <si>
     <t>All Forms</t>
   </si>
   <si>
-    <t>Form3 (manage)</t>
-  </si>
-  <si>
     <t>6 to 8</t>
   </si>
   <si>
@@ -155,12 +149,6 @@
     <t>Create entry points to Form3</t>
   </si>
   <si>
-    <t>Form3 (manage) + Form4 (pass generation) ?</t>
-  </si>
-  <si>
-    <t>Form4 (pass generation)</t>
-  </si>
-  <si>
     <t>There will be 2 buttons beside each login pair in Form2 - Edit and Delete. There will also be a big button somewhere to create a new pair. You can make the editing UI the same as creating but has already the fields populated with current data</t>
   </si>
   <si>
@@ -201,6 +189,21 @@
   </si>
   <si>
     <t>6 to 9</t>
+  </si>
+  <si>
+    <t>Form3 (main)</t>
+  </si>
+  <si>
+    <t>Form2 (Register) + Form4 (manage) + Form5 (pass generation) ?</t>
+  </si>
+  <si>
+    <t>Form5 (pass generation)</t>
+  </si>
+  <si>
+    <t>Form4 (manage)</t>
+  </si>
+  <si>
+    <t>Form1 (login) + Form2 (register)</t>
   </si>
 </sst>
 </file>
@@ -238,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,12 +269,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -368,10 +365,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -379,34 +379,14 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
-          <xfpb:xfComplement i="0"/>
-        </ext>
-      </extLst>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -416,10 +396,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF99"/>
       <color rgb="FFCC99FF"/>
       <color rgb="FFCCFFFF"/>
       <color rgb="FFCC9900"/>
-      <color rgb="FFFFFF99"/>
     </mruColors>
   </colors>
   <extLst>
@@ -769,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C283816F-F95C-444B-A286-FFF884AAF55E}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,13 +784,13 @@
         <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -818,31 +798,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="7">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>46</v>
+        <v>28</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -850,7 +830,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="9" t="b">
         <v>0</v>
@@ -859,22 +839,22 @@
         <v>6.5</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="F3" s="10">
         <v>1</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="4" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
@@ -882,31 +862,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="9" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="F4" s="10">
         <v>3</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -914,7 +894,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="6" t="b">
         <v>0</v>
@@ -923,22 +903,22 @@
         <v>6</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="F5" s="7">
         <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="20" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -946,7 +926,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="6" t="b">
         <v>0</v>
@@ -955,52 +935,52 @@
         <v>6</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="F6" s="7">
         <v>2</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>51</v>
+        <v>32</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="24" t="b">
+      <c r="B7" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="19" t="b">
         <v>0</v>
       </c>
       <c r="D7" s="11">
         <v>6.5</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F7" s="11">
         <v>4</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="26" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="4" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -1008,91 +988,95 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="13" t="b">
         <v>0</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="14">
         <v>5</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="18" t="b">
+      <c r="B9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="7">
         <v>5</v>
       </c>
-      <c r="E9" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="19">
+      <c r="E9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="7">
         <v>3</v>
       </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="21" t="s">
-        <v>49</v>
+      <c r="G9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="18" t="b">
+      <c r="B10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="13" t="b">
         <v>0</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="19">
+        <v>49</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="14">
         <v>2</v>
       </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="21" t="s">
-        <v>50</v>
+      <c r="G10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1100,7 +1084,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="13" t="b">
         <v>0</v>
@@ -1108,53 +1092,53 @@
       <c r="D11" s="14">
         <v>7</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>39</v>
+      <c r="E11" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="F11" s="14">
         <v>4</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="24" t="b">
+      <c r="B12" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="19" t="b">
         <v>0</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="20" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" s="11">
         <v>5</v>
       </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="26" t="s">
-        <v>52</v>
+        <v>32</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>